<commit_message>
Switch to Google Sheets and New Firebase
</commit_message>
<xml_diff>
--- a/dashboard_CoE .xlsx
+++ b/dashboard_CoE .xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10102"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10125"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/santaclaus/Desktop/BNCT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53B1C2D7-B54B-E64A-BE56-37136155C092}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F6326BB-33E2-E849-A9B1-AC5101057396}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15720" xr2:uid="{C2E5A323-D79E-449A-BCCD-EA9358631BAB}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{C2E5A323-D79E-449A-BCCD-EA9358631BAB}"/>
   </bookViews>
   <sheets>
     <sheet name="Format" sheetId="12" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="704" uniqueCount="225">
   <si>
     <t>C01</t>
   </si>
@@ -781,6 +781,15 @@
   </si>
   <si>
     <t>10. ข้อเสนอแนะเชิงนโยบาย (Policy Recommendation) และมาตรการ (Measures)</t>
+  </si>
+  <si>
+    <t>ใช้แล้ว</t>
+  </si>
+  <si>
+    <t>คงเหลือ</t>
+  </si>
+  <si>
+    <t>9/30/2567</t>
   </si>
 </sst>
 </file>
@@ -945,12 +954,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="65"/>
       </patternFill>
@@ -965,6 +968,12 @@
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -1139,7 +1148,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1150,9 +1159,8 @@
     <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1211,28 +1219,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="9" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="8" applyBorder="1"/>
     <xf numFmtId="14" fontId="9" fillId="6" borderId="1" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="7" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="11" borderId="1" xfId="8" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="13" borderId="1" xfId="10" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="12" borderId="1" xfId="9" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="8" borderId="14" xfId="5" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="9" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="8" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="13" borderId="1" xfId="10" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="12" borderId="1" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1253,12 +1258,15 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="9" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="10">
     <cellStyle name="20% - Accent2" xfId="7" builtinId="34"/>
-    <cellStyle name="20% - Accent3" xfId="8" builtinId="38"/>
-    <cellStyle name="20% - Accent4" xfId="9" builtinId="42"/>
-    <cellStyle name="20% - Accent5" xfId="10" builtinId="46"/>
+    <cellStyle name="20% - Accent4" xfId="8" builtinId="42"/>
+    <cellStyle name="20% - Accent5" xfId="9" builtinId="46"/>
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
     <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
@@ -1599,8 +1607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{471E291B-9F9E-45FD-BD8D-FA3BB484E07E}">
   <dimension ref="A1:Q56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1617,60 +1625,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="20" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="40" t="s">
+      <c r="C1" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="40" t="s">
+      <c r="D1" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="40" t="s">
+      <c r="E1" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="40" t="s">
+      <c r="F1" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="40" t="s">
+      <c r="G1" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="40" t="s">
+      <c r="H1" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="40" t="s">
+      <c r="I1" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="40" t="s">
+      <c r="J1" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="40" t="s">
+      <c r="K1" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="40" t="s">
+      <c r="L1" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="40" t="s">
+      <c r="M1" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="40" t="s">
+      <c r="N1" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="40" t="s">
+      <c r="O1" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="40" t="s">
+      <c r="P1" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="40" t="s">
+      <c r="Q1" s="39" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="38" t="s">
         <v>17</v>
       </c>
       <c r="B2" t="s">
@@ -1731,8 +1739,8 @@
       <c r="D6" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="37">
-        <v>243263</v>
+      <c r="E6" s="50" t="s">
+        <v>224</v>
       </c>
       <c r="F6" s="30" t="s">
         <v>29</v>
@@ -1743,13 +1751,13 @@
       <c r="H6" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="I6" s="38" t="s">
+      <c r="I6" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="J6" s="43" t="s">
+      <c r="J6" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="K6" s="43" t="s">
+      <c r="K6" s="42" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1771,6 +1779,19 @@
       </c>
       <c r="C8" s="31" t="s">
         <v>37</v>
+      </c>
+      <c r="D8" t="s">
+        <v>222</v>
+      </c>
+      <c r="E8">
+        <v>765467</v>
+      </c>
+      <c r="F8" t="s">
+        <v>223</v>
+      </c>
+      <c r="G8">
+        <f>B8-E8</f>
+        <v>9234532</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
@@ -1877,34 +1898,34 @@
       <c r="G13" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="H13" s="41" t="s">
+      <c r="H13" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="I13" s="41" t="s">
+      <c r="I13" s="40" t="s">
         <v>49</v>
       </c>
-      <c r="J13" s="41" t="s">
+      <c r="J13" s="40" t="s">
         <v>50</v>
       </c>
-      <c r="K13" s="41" t="s">
+      <c r="K13" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="L13" s="41" t="s">
+      <c r="L13" s="40" t="s">
         <v>52</v>
       </c>
-      <c r="M13" s="41" t="s">
+      <c r="M13" s="40" t="s">
         <v>53</v>
       </c>
-      <c r="N13" s="41" t="s">
+      <c r="N13" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="O13" s="41" t="s">
+      <c r="O13" s="40" t="s">
         <v>55</v>
       </c>
-      <c r="P13" s="41" t="s">
+      <c r="P13" s="40" t="s">
         <v>56</v>
       </c>
-      <c r="Q13" s="41" t="s">
+      <c r="Q13" s="40" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1927,34 +1948,34 @@
       <c r="G14" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="H14" s="41" t="s">
+      <c r="H14" s="40" t="s">
         <v>59</v>
       </c>
-      <c r="I14" s="41" t="s">
+      <c r="I14" s="40" t="s">
         <v>60</v>
       </c>
-      <c r="J14" s="41" t="s">
+      <c r="J14" s="40" t="s">
         <v>61</v>
       </c>
-      <c r="K14" s="41" t="s">
+      <c r="K14" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="L14" s="41" t="s">
+      <c r="L14" s="40" t="s">
         <v>63</v>
       </c>
-      <c r="M14" s="41" t="s">
+      <c r="M14" s="40" t="s">
         <v>64</v>
       </c>
-      <c r="N14" s="41" t="s">
+      <c r="N14" s="40" t="s">
         <v>65</v>
       </c>
-      <c r="O14" s="41" t="s">
+      <c r="O14" s="40" t="s">
         <v>66</v>
       </c>
-      <c r="P14" s="41" t="s">
+      <c r="P14" s="40" t="s">
         <v>67</v>
       </c>
-      <c r="Q14" s="41" t="s">
+      <c r="Q14" s="40" t="s">
         <v>68</v>
       </c>
     </row>
@@ -1977,7 +1998,7 @@
       <c r="G15" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="H15" s="41" t="s">
+      <c r="H15" s="40" t="s">
         <v>48</v>
       </c>
       <c r="I15" s="34" t="s">
@@ -3084,60 +3105,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="20" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="40" t="s">
+      <c r="C1" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="40" t="s">
+      <c r="D1" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="40" t="s">
+      <c r="E1" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="40" t="s">
+      <c r="F1" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="40" t="s">
+      <c r="G1" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="40" t="s">
+      <c r="H1" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="40" t="s">
+      <c r="I1" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="40" t="s">
+      <c r="J1" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="40" t="s">
+      <c r="K1" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="40" t="s">
+      <c r="L1" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="40" t="s">
+      <c r="M1" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="40" t="s">
+      <c r="N1" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="40" t="s">
+      <c r="O1" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="40" t="s">
+      <c r="P1" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="40" t="s">
+      <c r="Q1" s="39" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="38" t="s">
         <v>17</v>
       </c>
       <c r="B2" t="s">
@@ -3198,25 +3219,25 @@
       <c r="D6" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="37">
-        <v>243263</v>
+      <c r="E6" s="35" t="s">
+        <v>224</v>
       </c>
       <c r="F6" s="30" t="s">
         <v>29</v>
       </c>
       <c r="G6" s="35" t="s">
-        <v>30</v>
+        <v>224</v>
       </c>
       <c r="H6" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="I6" s="38" t="s">
+      <c r="I6" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="J6" s="43" t="s">
+      <c r="J6" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="K6" s="43" t="s">
+      <c r="K6" s="42" t="s">
         <v>34</v>
       </c>
     </row>
@@ -3238,6 +3259,19 @@
       </c>
       <c r="C8" s="31" t="s">
         <v>37</v>
+      </c>
+      <c r="D8" t="s">
+        <v>222</v>
+      </c>
+      <c r="E8" s="49">
+        <v>54321</v>
+      </c>
+      <c r="F8" t="s">
+        <v>223</v>
+      </c>
+      <c r="G8" s="49">
+        <f>B8-E8</f>
+        <v>3145679</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
@@ -3344,34 +3378,34 @@
       <c r="G13" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="H13" s="41" t="s">
+      <c r="H13" s="40" t="s">
         <v>119</v>
       </c>
-      <c r="I13" s="41" t="s">
+      <c r="I13" s="40" t="s">
         <v>120</v>
       </c>
-      <c r="J13" s="41" t="s">
+      <c r="J13" s="40" t="s">
         <v>121</v>
       </c>
-      <c r="K13" s="41" t="s">
+      <c r="K13" s="40" t="s">
         <v>122</v>
       </c>
-      <c r="L13" s="41" t="s">
+      <c r="L13" s="40" t="s">
         <v>123</v>
       </c>
-      <c r="M13" s="41" t="s">
+      <c r="M13" s="40" t="s">
         <v>124</v>
       </c>
-      <c r="N13" s="41" t="s">
+      <c r="N13" s="40" t="s">
         <v>125</v>
       </c>
-      <c r="O13" s="41" t="s">
+      <c r="O13" s="40" t="s">
         <v>126</v>
       </c>
-      <c r="P13" s="41" t="s">
+      <c r="P13" s="40" t="s">
         <v>127</v>
       </c>
-      <c r="Q13" s="41" t="s">
+      <c r="Q13" s="40" t="s">
         <v>128</v>
       </c>
     </row>
@@ -3394,31 +3428,31 @@
       <c r="G14" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="H14" s="41" t="s">
+      <c r="H14" s="40" t="s">
         <v>129</v>
       </c>
-      <c r="I14" s="41" t="s">
+      <c r="I14" s="40" t="s">
         <v>130</v>
       </c>
-      <c r="J14" s="41" t="s">
+      <c r="J14" s="40" t="s">
         <v>131</v>
       </c>
-      <c r="K14" s="41" t="s">
+      <c r="K14" s="40" t="s">
         <v>132</v>
       </c>
-      <c r="L14" s="41" t="s">
+      <c r="L14" s="40" t="s">
         <v>133</v>
       </c>
-      <c r="M14" s="41" t="s">
+      <c r="M14" s="40" t="s">
         <v>134</v>
       </c>
-      <c r="N14" s="41" t="s">
+      <c r="N14" s="40" t="s">
         <v>135</v>
       </c>
-      <c r="O14" s="41" t="s">
+      <c r="O14" s="40" t="s">
         <v>136</v>
       </c>
-      <c r="P14" s="41" t="s">
+      <c r="P14" s="40" t="s">
         <v>137</v>
       </c>
       <c r="Q14" s="34"/>
@@ -3442,28 +3476,28 @@
       <c r="G15" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="H15" s="41" t="s">
+      <c r="H15" s="40" t="s">
         <v>137</v>
       </c>
-      <c r="I15" s="41" t="s">
+      <c r="I15" s="40" t="s">
         <v>132</v>
       </c>
-      <c r="J15" s="41" t="s">
+      <c r="J15" s="40" t="s">
         <v>134</v>
       </c>
-      <c r="K15" s="41" t="s">
+      <c r="K15" s="40" t="s">
         <v>138</v>
       </c>
-      <c r="L15" s="41" t="s">
+      <c r="L15" s="40" t="s">
         <v>133</v>
       </c>
-      <c r="M15" s="41" t="s">
+      <c r="M15" s="40" t="s">
         <v>139</v>
       </c>
-      <c r="N15" s="41" t="s">
+      <c r="N15" s="40" t="s">
         <v>140</v>
       </c>
-      <c r="O15" s="41" t="s">
+      <c r="O15" s="40" t="s">
         <v>141</v>
       </c>
       <c r="P15" s="34"/>
@@ -3488,15 +3522,15 @@
       <c r="G16" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="H16" s="41" t="s">
+      <c r="H16" s="40" t="s">
         <v>142</v>
       </c>
-      <c r="I16" s="41" t="s">
+      <c r="I16" s="40" t="s">
         <v>143</v>
       </c>
       <c r="J16" s="34"/>
       <c r="K16" s="34"/>
-      <c r="L16" s="41"/>
+      <c r="L16" s="40"/>
       <c r="M16" s="34"/>
       <c r="N16" s="34"/>
       <c r="O16" s="34"/>
@@ -3663,20 +3697,20 @@
       <c r="G22" s="25" t="s">
         <v>85</v>
       </c>
-      <c r="H22" s="41" t="s">
+      <c r="H22" s="40" t="s">
         <v>144</v>
       </c>
-      <c r="I22" s="41" t="s">
+      <c r="I22" s="40" t="s">
         <v>145</v>
       </c>
-      <c r="J22" s="41" t="s">
+      <c r="J22" s="40" t="s">
         <v>146</v>
       </c>
-      <c r="K22" s="41" t="s">
+      <c r="K22" s="40" t="s">
         <v>147</v>
       </c>
       <c r="L22" s="34"/>
-      <c r="M22" s="41"/>
+      <c r="M22" s="40"/>
       <c r="N22" s="34"/>
       <c r="O22" s="34"/>
       <c r="P22" s="34"/>
@@ -3701,22 +3735,22 @@
       <c r="G23" s="25" t="s">
         <v>85</v>
       </c>
-      <c r="H23" s="41" t="s">
+      <c r="H23" s="40" t="s">
         <v>148</v>
       </c>
-      <c r="I23" s="41" t="s">
+      <c r="I23" s="40" t="s">
         <v>149</v>
       </c>
-      <c r="J23" s="41" t="s">
+      <c r="J23" s="40" t="s">
         <v>150</v>
       </c>
-      <c r="K23" s="41" t="s">
+      <c r="K23" s="40" t="s">
         <v>151</v>
       </c>
-      <c r="L23" s="41" t="s">
+      <c r="L23" s="40" t="s">
         <v>152</v>
       </c>
-      <c r="M23" s="41" t="s">
+      <c r="M23" s="40" t="s">
         <v>153</v>
       </c>
       <c r="N23" s="34"/>
@@ -3991,7 +4025,7 @@
       <c r="G33" s="25" t="s">
         <v>98</v>
       </c>
-      <c r="H33" s="41" t="s">
+      <c r="H33" s="40" t="s">
         <v>154</v>
       </c>
       <c r="I33" s="34"/>
@@ -4023,7 +4057,7 @@
       <c r="G34" s="25" t="s">
         <v>98</v>
       </c>
-      <c r="H34" s="41" t="s">
+      <c r="H34" s="40" t="s">
         <v>155</v>
       </c>
       <c r="I34" s="34"/>
@@ -4499,8 +4533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95087F74-347A-4E12-AC65-69C0B5898E3A}">
   <dimension ref="A1:Q56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4517,60 +4551,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="20" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="40" t="s">
+      <c r="C1" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="40" t="s">
+      <c r="D1" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="40" t="s">
+      <c r="E1" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="40" t="s">
+      <c r="F1" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="40" t="s">
+      <c r="G1" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="40" t="s">
+      <c r="H1" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="40" t="s">
+      <c r="I1" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="40" t="s">
+      <c r="J1" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="40" t="s">
+      <c r="K1" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="40" t="s">
+      <c r="L1" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="40" t="s">
+      <c r="M1" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="40" t="s">
+      <c r="N1" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="40" t="s">
+      <c r="O1" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="40" t="s">
+      <c r="P1" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="40" t="s">
+      <c r="Q1" s="39" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="38" t="s">
         <v>17</v>
       </c>
       <c r="B2" t="s">
@@ -4605,10 +4639,10 @@
       <c r="I5" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="J5" s="42" t="s">
+      <c r="J5" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="K5" s="42" t="s">
+      <c r="K5" s="41" t="s">
         <v>25</v>
       </c>
       <c r="L5" s="33"/>
@@ -4631,8 +4665,8 @@
       <c r="D6" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="37">
-        <v>243628</v>
+      <c r="E6" s="50" t="s">
+        <v>224</v>
       </c>
       <c r="F6" s="30" t="s">
         <v>29</v>
@@ -4643,13 +4677,13 @@
       <c r="H6" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="I6" s="38" t="s">
+      <c r="I6" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="J6" s="38" t="s">
+      <c r="J6" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="K6" s="38" t="s">
+      <c r="K6" s="37" t="s">
         <v>158</v>
       </c>
     </row>
@@ -4671,6 +4705,19 @@
       </c>
       <c r="C8" s="31" t="s">
         <v>37</v>
+      </c>
+      <c r="D8" t="s">
+        <v>222</v>
+      </c>
+      <c r="E8">
+        <v>12345</v>
+      </c>
+      <c r="F8" t="s">
+        <v>223</v>
+      </c>
+      <c r="G8">
+        <f>B8-E8</f>
+        <v>3187655</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
@@ -4777,34 +4824,34 @@
       <c r="G13" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="H13" s="41" t="s">
+      <c r="H13" s="40" t="s">
         <v>119</v>
       </c>
-      <c r="I13" s="41" t="s">
+      <c r="I13" s="40" t="s">
         <v>120</v>
       </c>
-      <c r="J13" s="41" t="s">
+      <c r="J13" s="40" t="s">
         <v>121</v>
       </c>
-      <c r="K13" s="41" t="s">
+      <c r="K13" s="40" t="s">
         <v>122</v>
       </c>
-      <c r="L13" s="41" t="s">
+      <c r="L13" s="40" t="s">
         <v>159</v>
       </c>
-      <c r="M13" s="41" t="s">
+      <c r="M13" s="40" t="s">
         <v>160</v>
       </c>
-      <c r="N13" s="41" t="s">
+      <c r="N13" s="40" t="s">
         <v>125</v>
       </c>
-      <c r="O13" s="41" t="s">
+      <c r="O13" s="40" t="s">
         <v>126</v>
       </c>
-      <c r="P13" s="41" t="s">
+      <c r="P13" s="40" t="s">
         <v>127</v>
       </c>
-      <c r="Q13" s="41" t="s">
+      <c r="Q13" s="40" t="s">
         <v>128</v>
       </c>
     </row>
@@ -4827,31 +4874,31 @@
       <c r="G14" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="H14" s="41" t="s">
+      <c r="H14" s="40" t="s">
         <v>129</v>
       </c>
-      <c r="I14" s="41" t="s">
+      <c r="I14" s="40" t="s">
         <v>130</v>
       </c>
-      <c r="J14" s="41" t="s">
+      <c r="J14" s="40" t="s">
         <v>131</v>
       </c>
-      <c r="K14" s="41" t="s">
+      <c r="K14" s="40" t="s">
         <v>132</v>
       </c>
-      <c r="L14" s="41" t="s">
+      <c r="L14" s="40" t="s">
         <v>133</v>
       </c>
-      <c r="M14" s="41" t="s">
+      <c r="M14" s="40" t="s">
         <v>161</v>
       </c>
-      <c r="N14" s="41" t="s">
+      <c r="N14" s="40" t="s">
         <v>135</v>
       </c>
-      <c r="O14" s="41" t="s">
+      <c r="O14" s="40" t="s">
         <v>136</v>
       </c>
-      <c r="P14" s="41" t="s">
+      <c r="P14" s="40" t="s">
         <v>137</v>
       </c>
       <c r="Q14" s="34"/>
@@ -4875,28 +4922,28 @@
       <c r="G15" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="H15" s="41" t="s">
+      <c r="H15" s="40" t="s">
         <v>137</v>
       </c>
-      <c r="I15" s="41" t="s">
+      <c r="I15" s="40" t="s">
         <v>132</v>
       </c>
-      <c r="J15" s="41" t="s">
+      <c r="J15" s="40" t="s">
         <v>134</v>
       </c>
-      <c r="K15" s="41" t="s">
+      <c r="K15" s="40" t="s">
         <v>138</v>
       </c>
-      <c r="L15" s="41" t="s">
+      <c r="L15" s="40" t="s">
         <v>133</v>
       </c>
-      <c r="M15" s="41" t="s">
+      <c r="M15" s="40" t="s">
         <v>139</v>
       </c>
-      <c r="N15" s="41" t="s">
+      <c r="N15" s="40" t="s">
         <v>140</v>
       </c>
-      <c r="O15" s="41" t="s">
+      <c r="O15" s="40" t="s">
         <v>141</v>
       </c>
       <c r="P15" s="34"/>
@@ -4923,15 +4970,15 @@
       <c r="G16" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="H16" s="41" t="s">
+      <c r="H16" s="40" t="s">
         <v>142</v>
       </c>
-      <c r="I16" s="41" t="s">
+      <c r="I16" s="40" t="s">
         <v>143</v>
       </c>
       <c r="J16" s="34"/>
       <c r="K16" s="34"/>
-      <c r="L16" s="41"/>
+      <c r="L16" s="40"/>
       <c r="M16" s="34"/>
       <c r="N16" s="34"/>
       <c r="O16" s="34"/>
@@ -5098,20 +5145,20 @@
       <c r="G22" s="25" t="s">
         <v>85</v>
       </c>
-      <c r="H22" s="41" t="s">
+      <c r="H22" s="40" t="s">
         <v>144</v>
       </c>
-      <c r="I22" s="41" t="s">
+      <c r="I22" s="40" t="s">
         <v>145</v>
       </c>
-      <c r="J22" s="41" t="s">
+      <c r="J22" s="40" t="s">
         <v>146</v>
       </c>
-      <c r="K22" s="41" t="s">
+      <c r="K22" s="40" t="s">
         <v>147</v>
       </c>
       <c r="L22" s="34"/>
-      <c r="M22" s="41"/>
+      <c r="M22" s="40"/>
       <c r="N22" s="34"/>
       <c r="O22" s="34"/>
       <c r="P22" s="34"/>
@@ -5136,22 +5183,22 @@
       <c r="G23" s="25" t="s">
         <v>85</v>
       </c>
-      <c r="H23" s="41" t="s">
+      <c r="H23" s="40" t="s">
         <v>148</v>
       </c>
-      <c r="I23" s="41" t="s">
+      <c r="I23" s="40" t="s">
         <v>149</v>
       </c>
-      <c r="J23" s="41" t="s">
+      <c r="J23" s="40" t="s">
         <v>150</v>
       </c>
-      <c r="K23" s="41" t="s">
+      <c r="K23" s="40" t="s">
         <v>151</v>
       </c>
-      <c r="L23" s="41" t="s">
+      <c r="L23" s="40" t="s">
         <v>152</v>
       </c>
-      <c r="M23" s="41" t="s">
+      <c r="M23" s="40" t="s">
         <v>153</v>
       </c>
       <c r="N23" s="34"/>
@@ -5426,7 +5473,7 @@
       <c r="G33" s="25" t="s">
         <v>98</v>
       </c>
-      <c r="H33" s="41" t="s">
+      <c r="H33" s="40" t="s">
         <v>154</v>
       </c>
       <c r="I33" s="34"/>
@@ -5458,7 +5505,7 @@
       <c r="G34" s="25" t="s">
         <v>98</v>
       </c>
-      <c r="H34" s="41" t="s">
+      <c r="H34" s="40" t="s">
         <v>155</v>
       </c>
       <c r="I34" s="34"/>
@@ -6061,13 +6108,13 @@
       <c r="J8" s="13"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A9" s="46" t="s">
+      <c r="A9" s="45" t="s">
         <v>168</v>
       </c>
-      <c r="B9" s="47"/>
-      <c r="C9" s="47"/>
-      <c r="D9" s="47"/>
-      <c r="E9" s="47"/>
+      <c r="B9" s="46"/>
+      <c r="C9" s="46"/>
+      <c r="D9" s="46"/>
+      <c r="E9" s="46"/>
       <c r="J9" s="13"/>
       <c r="K9" s="1" t="s">
         <v>169</v>
@@ -6195,13 +6242,13 @@
       <c r="J17" s="13"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A18" s="46" t="s">
+      <c r="A18" s="45" t="s">
         <v>175</v>
       </c>
-      <c r="B18" s="47"/>
-      <c r="C18" s="47"/>
-      <c r="D18" s="47"/>
-      <c r="E18" s="47"/>
+      <c r="B18" s="46"/>
+      <c r="C18" s="46"/>
+      <c r="D18" s="46"/>
+      <c r="E18" s="46"/>
       <c r="J18" s="13"/>
       <c r="K18" s="1" t="s">
         <v>85</v>
@@ -6317,13 +6364,13 @@
       <c r="J25" s="13"/>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A26" s="46" t="s">
+      <c r="A26" s="45" t="s">
         <v>186</v>
       </c>
-      <c r="B26" s="47"/>
-      <c r="C26" s="47"/>
-      <c r="D26" s="47"/>
-      <c r="E26" s="47"/>
+      <c r="B26" s="46"/>
+      <c r="C26" s="46"/>
+      <c r="D26" s="46"/>
+      <c r="E26" s="46"/>
       <c r="J26" s="13"/>
       <c r="K26" s="1" t="s">
         <v>94</v>
@@ -6367,13 +6414,13 @@
       <c r="J28" s="13"/>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A29" s="46" t="s">
+      <c r="A29" s="45" t="s">
         <v>192</v>
       </c>
-      <c r="B29" s="47"/>
-      <c r="C29" s="47"/>
-      <c r="D29" s="47"/>
-      <c r="E29" s="47"/>
+      <c r="B29" s="46"/>
+      <c r="C29" s="46"/>
+      <c r="D29" s="46"/>
+      <c r="E29" s="46"/>
       <c r="J29" s="13"/>
       <c r="K29" s="1" t="s">
         <v>98</v>
@@ -6445,13 +6492,13 @@
       <c r="J33" s="13"/>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A34" s="46" t="s">
+      <c r="A34" s="45" t="s">
         <v>201</v>
       </c>
-      <c r="B34" s="47"/>
-      <c r="C34" s="47"/>
-      <c r="D34" s="47"/>
-      <c r="E34" s="47"/>
+      <c r="B34" s="46"/>
+      <c r="C34" s="46"/>
+      <c r="D34" s="46"/>
+      <c r="E34" s="46"/>
       <c r="J34" s="13"/>
       <c r="K34" s="1" t="s">
         <v>103</v>
@@ -6495,13 +6542,13 @@
       <c r="J36" s="13"/>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A37" s="46" t="s">
+      <c r="A37" s="45" t="s">
         <v>207</v>
       </c>
-      <c r="B37" s="47"/>
-      <c r="C37" s="47"/>
-      <c r="D37" s="47"/>
-      <c r="E37" s="47"/>
+      <c r="B37" s="46"/>
+      <c r="C37" s="46"/>
+      <c r="D37" s="46"/>
+      <c r="E37" s="46"/>
       <c r="J37" s="13"/>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.4">
@@ -6521,13 +6568,13 @@
       <c r="J39" s="13"/>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A40" s="44" t="s">
+      <c r="A40" s="43" t="s">
         <v>208</v>
       </c>
-      <c r="B40" s="45"/>
-      <c r="C40" s="45"/>
-      <c r="D40" s="45"/>
-      <c r="E40" s="45"/>
+      <c r="B40" s="44"/>
+      <c r="C40" s="44"/>
+      <c r="D40" s="44"/>
+      <c r="E40" s="44"/>
       <c r="J40" s="13"/>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.4">
@@ -6551,13 +6598,13 @@
       <c r="J42" s="13"/>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A43" s="44" t="s">
+      <c r="A43" s="43" t="s">
         <v>209</v>
       </c>
-      <c r="B43" s="45"/>
-      <c r="C43" s="45"/>
-      <c r="D43" s="45"/>
-      <c r="E43" s="45"/>
+      <c r="B43" s="44"/>
+      <c r="C43" s="44"/>
+      <c r="D43" s="44"/>
+      <c r="E43" s="44"/>
       <c r="J43" s="13"/>
       <c r="K43" s="1" t="s">
         <v>110</v>
@@ -6615,13 +6662,13 @@
       <c r="J46" s="13"/>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A47" s="46" t="s">
+      <c r="A47" s="45" t="s">
         <v>215</v>
       </c>
-      <c r="B47" s="47"/>
-      <c r="C47" s="47"/>
-      <c r="D47" s="47"/>
-      <c r="E47" s="47"/>
+      <c r="B47" s="46"/>
+      <c r="C47" s="46"/>
+      <c r="D47" s="46"/>
+      <c r="E47" s="46"/>
       <c r="J47" s="13"/>
       <c r="K47" s="1" t="s">
         <v>115</v>
@@ -6679,13 +6726,13 @@
       <c r="J50" s="13"/>
     </row>
     <row r="51" spans="1:10" ht="20.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A51" s="48" t="s">
+      <c r="A51" s="47" t="s">
         <v>221</v>
       </c>
-      <c r="B51" s="49"/>
-      <c r="C51" s="49"/>
-      <c r="D51" s="49"/>
-      <c r="E51" s="49"/>
+      <c r="B51" s="48"/>
+      <c r="C51" s="48"/>
+      <c r="D51" s="48"/>
+      <c r="E51" s="48"/>
       <c r="J51" s="13"/>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.4">

</xml_diff>